<commit_message>
Updated BaseTest and DriverManager fixes
</commit_message>
<xml_diff>
--- a/LoginData.xlsx
+++ b/LoginData.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium Assignment\ecommerce-automation-framework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ecommerce-automation-framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD4359E-FB56-4F68-9308-5A341F560453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB71965A-CF05-460F-A7B3-71DA626330D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Login" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,35 +27,35 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>expectedResult</t>
-  </si>
-  <si>
     <t>standard_user</t>
   </si>
   <si>
     <t>secret_sauce</t>
   </si>
   <si>
-    <t>success</t>
-  </si>
-  <si>
     <t>locked_out_user</t>
   </si>
   <si>
-    <t>failure</t>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>ExpectedResult</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,20 +67,31 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -88,16 +99,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDDDDDD"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDDDDDD"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -383,7 +412,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:C5"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -393,36 +422,36 @@
     <col min="3" max="3" width="25.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>